<commit_message>
return book, but not working, because of some borrowed_books error
</commit_message>
<xml_diff>
--- a/library/data/books.xlsx
+++ b/library/data/books.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +468,41 @@
           <t>Pages</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lent</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lent to</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Lent date</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Return date</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Reserved</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Reserved by</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Reserved until</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -492,6 +531,25 @@
       <c r="F2" t="n">
         <v>292</v>
       </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>45805.66867783668</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>45835.66867783669</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" s="2" t="n">
+        <v>45805.659361875</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -519,6 +577,19 @@
       </c>
       <c r="F3" t="n">
         <v>584</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" s="2" t="n">
+        <v>45806.65936186343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reserve, extend and history
</commit_message>
<xml_diff>
--- a/library/data/books.xlsx
+++ b/library/data/books.xlsx
@@ -538,18 +538,16 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>45805.66867783668</v>
+        <v>45805.74464392842</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>45835.66867783669</v>
+        <v>45835.74464392842</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
       </c>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" s="2" t="n">
-        <v>45805.659361875</v>
-      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -588,9 +586,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" s="2" t="n">
-        <v>45806.65936186343</v>
-      </c>
+      <c r="M3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
returning books works now
</commit_message>
<xml_diff>
--- a/library/data/books.xlsx
+++ b/library/data/books.xlsx
@@ -532,24 +532,16 @@
         <v>292</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>45805.66867783668</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>45835.66867783669</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="b">
         <v>0</v>
       </c>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" s="2" t="n">
-        <v>45805.659361875</v>
-      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">

</xml_diff>